<commit_message>
Implemented firmware based on PLBv4.6, generated bitstream, and write a demo for the DAC driver in SDK
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academic\FPGA\BR0101\Development\DAC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programs\Verilog\FPGA_Group\test_br0101\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
     <sheet name="重要寄存器定义" sheetId="2" r:id="rId2"/>
+    <sheet name="固件寄存器格式" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>MSB</t>
   </si>
@@ -110,6 +111,56 @@
   </si>
   <si>
     <t>起始地址控制位</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b31 - b2</t>
+  </si>
+  <si>
+    <t>FRMT_CTL</t>
+  </si>
+  <si>
+    <t>备用</t>
+  </si>
+  <si>
+    <t>格式控制位，0表示无符号二进制数，
+1表示二进制补码，默认为0</t>
+  </si>
+  <si>
+    <t>DAC_EN</t>
+  </si>
+  <si>
+    <t>DAC使能控制位，为0时DAC掉电，为1时正常工作</t>
+  </si>
+  <si>
+    <t>reg0
+DAC_CTL
+DAC控制寄存器</t>
+  </si>
+  <si>
+    <t>reg1
+DAC_DATA
+DAC数据寄存器</t>
+  </si>
+  <si>
+    <t>b31-b10</t>
+  </si>
+  <si>
+    <t>b9-b0</t>
+  </si>
+  <si>
+    <t>DAC_DATABITS</t>
+  </si>
+  <si>
+    <t>DAC数据位</t>
   </si>
 </sst>
 </file>
@@ -175,11 +226,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -604,4 +661,111 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the firmware, allow interleaved access to I DAC and Q DAC
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
     <sheet name="重要寄存器定义" sheetId="2" r:id="rId2"/>
     <sheet name="固件寄存器格式" sheetId="3" r:id="rId3"/>
+    <sheet name="固件寄存器格式 - 修改" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>MSB</t>
   </si>
@@ -161,6 +162,30 @@
   </si>
   <si>
     <t>DAC数据位</t>
+  </si>
+  <si>
+    <t>b31-b26</t>
+  </si>
+  <si>
+    <t>b25-b16</t>
+  </si>
+  <si>
+    <t>DAC_Q_DATA</t>
+  </si>
+  <si>
+    <t>Q DAC数据位</t>
+  </si>
+  <si>
+    <t>b15-b10</t>
+  </si>
+  <si>
+    <t>格式控制位，0表示无符号二进制数，1表示二进制补码，默认为0</t>
+  </si>
+  <si>
+    <t>DAC_I_DATA</t>
+  </si>
+  <si>
+    <t>I DAC数据位</t>
   </si>
 </sst>
 </file>
@@ -226,18 +251,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -627,17 +653,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -667,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,7 +715,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -703,7 +729,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -715,45 +741,45 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -768,4 +794,131 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.5" customHeight="1">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Op Amp control signals, completed the UCF
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
     <sheet name="重要寄存器定义" sheetId="2" r:id="rId2"/>
     <sheet name="固件寄存器格式" sheetId="3" r:id="rId3"/>
     <sheet name="固件寄存器格式 - 修改" sheetId="4" r:id="rId4"/>
+    <sheet name="引脚约束" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>MSB</t>
   </si>
@@ -186,6 +187,150 @@
   </si>
   <si>
     <t>I DAC数据位</t>
+  </si>
+  <si>
+    <t>fpga_0_clk_1_sys_clk_pin</t>
+  </si>
+  <si>
+    <t>F18</t>
+  </si>
+  <si>
+    <t>LVCMOS33</t>
+  </si>
+  <si>
+    <t>fpga_0_RS232_TX_pin</t>
+  </si>
+  <si>
+    <t>USTTRIG</t>
+  </si>
+  <si>
+    <t>AG21</t>
+  </si>
+  <si>
+    <t>LVCMOS25</t>
+  </si>
+  <si>
+    <t>fpga_0_RS232_RX_pin</t>
+  </si>
+  <si>
+    <t>TDRSWITCH</t>
+  </si>
+  <si>
+    <t>AF20</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>G15</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_DCLKIO_pin</t>
+  </si>
+  <si>
+    <t>DAP1DCLKIO</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_Clkout_pin</t>
+  </si>
+  <si>
+    <t>DAP1CLKIN</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_PinMD_pin</t>
+  </si>
+  <si>
+    <t>DAP1RESET</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_ClkMD_pin</t>
+  </si>
+  <si>
+    <t>DAP1SCLK</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_Format_pin</t>
+  </si>
+  <si>
+    <t>DAP1SDIO</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_PWRDN_pin</t>
+  </si>
+  <si>
+    <t>DAP1CS</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_OpEnI_pin</t>
+  </si>
+  <si>
+    <t>ODAP1ID</t>
+  </si>
+  <si>
+    <t>AB12</t>
+  </si>
+  <si>
+    <t>plb_dac_0_S_OpEnQ_pin</t>
+  </si>
+  <si>
+    <t>ODAP1QD</t>
+  </si>
+  <si>
+    <t>AA8</t>
+  </si>
+  <si>
+    <t>LVCMOS15</t>
+  </si>
+  <si>
+    <t>fpga_0_rst_1_sys_rst_pin</t>
+  </si>
+  <si>
+    <t>D0501</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -257,13 +402,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -653,17 +798,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -715,7 +860,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -729,7 +874,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -741,7 +886,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -753,33 +898,33 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -800,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
@@ -824,7 +969,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -833,45 +978,45 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -882,11 +1027,11 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -897,11 +1042,11 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -921,4 +1066,549 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="51.42578125" customWidth="1"/>
+    <col min="9" max="9" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="str">
+        <f xml:space="preserve"> "Net " &amp; B2 &amp; " LOC = " &amp; D2 &amp; ";"</f>
+        <v>Net fpga_0_clk_1_sys_clk_pin LOC = F18;</v>
+      </c>
+      <c r="H2" t="str">
+        <f xml:space="preserve"> "Net " &amp; B2 &amp; " IOSTANDARD = " &amp; E2 &amp; ";"</f>
+        <v>Net fpga_0_clk_1_sys_clk_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G20" si="0" xml:space="preserve"> "Net " &amp; B3 &amp; " LOC = " &amp; D3 &amp; ";"</f>
+        <v>Net fpga_0_RS232_TX_pin LOC = AG21;</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H20" si="1" xml:space="preserve"> "Net " &amp; B3 &amp; " IOSTANDARD = " &amp; E3 &amp; ";"</f>
+        <v>Net fpga_0_RS232_TX_pin IOSTANDARD = LVCMOS25;</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Net fpga_0_RS232_RX_pin LOC = AF20;</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>Net fpga_0_RS232_RX_pin IOSTANDARD = LVCMOS25;</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="str">
+        <f>"plb_dac_0_S_Data_pin&lt;" &amp; TEXT(ROW() - 5,"0") &amp; "&gt;"</f>
+        <v>plb_dac_0_S_Data_pin&lt;0&gt;</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"DAP1DB" &amp; TEXT(14 - ROW(), "0")</f>
+        <v>DAP1DB9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;0&gt; LOC = G5;</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;0&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="str">
+        <f t="shared" ref="B6:B14" si="2">"plb_dac_0_S_Data_pin&lt;" &amp; TEXT(ROW() - 5,"0") &amp; "&gt;"</f>
+        <v>plb_dac_0_S_Data_pin&lt;1&gt;</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C14" si="3">"DAP1DB" &amp; TEXT(14 - ROW(), "0")</f>
+        <v>DAP1DB8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;1&gt; LOC = J14;</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;1&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;2&gt;</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;2&gt; LOC = G1;</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;2&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;3&gt;</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;3&gt; LOC = F1;</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;3&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;4&gt;</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;4&gt; LOC = E1;</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;4&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;5&gt;</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;5&gt; LOC = D1;</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;5&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;6&gt;</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;6&gt; LOC = D2;</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;6&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;7&gt;</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;7&gt; LOC = F3;</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;7&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;8&gt;</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;8&gt; LOC = F4;</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;8&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="str">
+        <f t="shared" si="2"/>
+        <v>plb_dac_0_S_Data_pin&lt;9&gt;</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="3"/>
+        <v>DAP1DB0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;9&gt; LOC = G15;</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Data_pin&lt;9&gt; IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_DCLKIO_pin LOC = M6;</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_DCLKIO_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Clkout_pin LOC = P5;</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Clkout_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_PinMD_pin LOC = M10;</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_PinMD_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_ClkMD_pin LOC = E2;</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_ClkMD_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_Format_pin LOC = J1;</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_Format_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>Net plb_dac_0_S_PWRDN_pin LOC = J2;</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>Net plb_dac_0_S_PWRDN_pin IOSTANDARD = LVCMOS33;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="str">
+        <f xml:space="preserve"> "Net " &amp; B21 &amp; " LOC = " &amp; D21 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnI_pin LOC = AB12;</v>
+      </c>
+      <c r="H21" t="str">
+        <f xml:space="preserve"> "Net " &amp; B21 &amp; " IOSTANDARD = " &amp; E21 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnI_pin IOSTANDARD = LVCMOS15;</v>
+      </c>
+      <c r="I21" t="str">
+        <f xml:space="preserve"> "Net " &amp; B21 &amp; " Drive = " &amp; F21 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnI_pin Drive = 2;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ref="G22" si="4" xml:space="preserve"> "Net " &amp; B22 &amp; " LOC = " &amp; D22 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnQ_pin LOC = AA8;</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" ref="H22" si="5" xml:space="preserve"> "Net " &amp; B22 &amp; " IOSTANDARD = " &amp; E22 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnQ_pin IOSTANDARD = LVCMOS15;</v>
+      </c>
+      <c r="I22" t="str">
+        <f xml:space="preserve"> "Net " &amp; B22 &amp; " Drive = " &amp; F22 &amp; ";"</f>
+        <v>Net plb_dac_0_S_OpEnQ_pin Drive = 2;</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" ref="G23:G24" si="6" xml:space="preserve"> "Net " &amp; B24 &amp; " LOC = " &amp; D24 &amp; ";"</f>
+        <v>Net fpga_0_rst_1_sys_rst_pin LOC = A5;</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" ref="H23:H24" si="7" xml:space="preserve"> "Net " &amp; B24 &amp; " IOSTANDARD = " &amp; E24 &amp; ";"</f>
+        <v>Net fpga_0_rst_1_sys_rst_pin IOSTANDARD = LVCMOS25;</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" ref="I23:I24" si="8" xml:space="preserve"> "Net " &amp; B24 &amp; " Drive = " &amp; F24 &amp; ";"</f>
+        <v>Net fpga_0_rst_1_sys_rst_pin Drive = 2;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Generated bitstreams for debugging, working on firmware 2.00
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -16,7 +16,8 @@
     <sheet name="重要寄存器定义" sheetId="2" r:id="rId2"/>
     <sheet name="固件寄存器格式" sheetId="3" r:id="rId3"/>
     <sheet name="固件寄存器格式 - 修改" sheetId="4" r:id="rId4"/>
-    <sheet name="引脚约束" sheetId="5" r:id="rId5"/>
+    <sheet name="固件寄存器格式2.00" sheetId="6" r:id="rId5"/>
+    <sheet name="引脚约束" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="139">
   <si>
     <t>MSB</t>
   </si>
@@ -433,6 +434,53 @@
   </si>
   <si>
     <t>AA9</t>
+  </si>
+  <si>
+    <t>SPI_STATE</t>
+  </si>
+  <si>
+    <t>reg2
+DAC_Q_DATA
+DAC Q数据寄存器</t>
+  </si>
+  <si>
+    <t>reg1
+DAC_I_DATA
+DAC I数据寄存器</t>
+  </si>
+  <si>
+    <t>b7-b0</t>
+  </si>
+  <si>
+    <t>b15-b8</t>
+  </si>
+  <si>
+    <t>SPI_DATA</t>
+  </si>
+  <si>
+    <t>SPI_INSTR</t>
+  </si>
+  <si>
+    <t>SPI指令</t>
+  </si>
+  <si>
+    <t>SPI数据</t>
+  </si>
+  <si>
+    <t>reg4
+DAC_SPI_DATA
+DAC SPI数据寄存器</t>
+  </si>
+  <si>
+    <t>reg3
+DAC_SPI_INSTR
+DAC SPI指令寄存器</t>
+  </si>
+  <si>
+    <t>I_DATA</t>
+  </si>
+  <si>
+    <t>Q_DATA</t>
   </si>
 </sst>
 </file>
@@ -471,7 +519,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -494,11 +542,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -510,6 +584,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,9 +1258,243 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="135" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="E12" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="E13" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="E16" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="G23" sqref="G23:I40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Simple SPI controller implemented, simulated alone
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
   <si>
     <t>MSB</t>
   </si>
@@ -481,6 +481,18 @@
   </si>
   <si>
     <t>Q_DATA</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>OpEnI</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>OpEnQ</t>
   </si>
 </sst>
 </file>
@@ -586,16 +598,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1260,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1291,26 +1303,38 @@
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="135" customHeight="1">
       <c r="A4" s="5"/>
@@ -1318,10 +1342,10 @@
         <v>26</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
@@ -1424,8 +1448,11 @@
         <v>22</v>
       </c>
       <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1434,8 +1461,11 @@
         <v>26</v>
       </c>
       <c r="C13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1461,9 +1491,6 @@
         <v>22</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="E15" s="1" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5"/>
@@ -1471,9 +1498,6 @@
         <v>26</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="E16" s="1" t="s">
-        <v>134</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Utilized and simulated plb_dac_2_00_a within MicroBlaze
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:I40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated documents about SPI
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="148">
   <si>
     <t>MSB</t>
   </si>
@@ -467,32 +467,46 @@
     <t>SPI数据</t>
   </si>
   <si>
+    <t>I_DATA</t>
+  </si>
+  <si>
+    <t>Q_DATA</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>OpEnI</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>OpEnQ</t>
+  </si>
+  <si>
+    <t>b31 - b4</t>
+  </si>
+  <si>
+    <t>b31-b16</t>
+  </si>
+  <si>
     <t>reg4
-DAC_SPI_DATA
-DAC SPI数据寄存器</t>
+BACKUP备用寄存器</t>
+  </si>
+  <si>
+    <t>Q运放控制</t>
+  </si>
+  <si>
+    <t>I运放控制</t>
+  </si>
+  <si>
+    <t>SPI状态标志</t>
   </si>
   <si>
     <t>reg3
-DAC_SPI_INSTR
-DAC SPI指令寄存器</t>
-  </si>
-  <si>
-    <t>I_DATA</t>
-  </si>
-  <si>
-    <t>Q_DATA</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>OpEnI</t>
-  </si>
-  <si>
-    <t>b3</t>
-  </si>
-  <si>
-    <t>OpEnQ</t>
+DAC_SPI
+DAC SPI寄存器</t>
   </si>
 </sst>
 </file>
@@ -531,7 +545,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -554,37 +568,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -595,18 +583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1272,17 +1248,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1290,6 +1268,9 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
@@ -1300,207 +1281,252 @@
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
         <v>139</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="s">
         <v>140</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" ht="135" customHeight="1">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="5"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="8" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="C6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="C9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5"/>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="26">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:A4"/>
@@ -1509,6 +1535,14 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1518,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Documents about debugging and waveform testing added
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="172">
   <si>
     <t>MSB</t>
   </si>
@@ -510,18 +510,9 @@
 DAC SPI寄存器</t>
   </si>
   <si>
-    <t>b4</t>
-  </si>
-  <si>
-    <t>b5</t>
-  </si>
-  <si>
     <t>WAV_FORM</t>
   </si>
   <si>
-    <t>波形控制</t>
-  </si>
-  <si>
     <t>b31 - b6</t>
   </si>
   <si>
@@ -537,30 +528,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>Depends on DAC_DATA</t>
-  </si>
-  <si>
-    <t>Rectanglar Wav</t>
-  </si>
-  <si>
-    <t>Sine Wave</t>
-  </si>
-  <si>
-    <t>I_WAV_FORM</t>
-  </si>
-  <si>
-    <t>D_WAV_FORM</t>
-  </si>
-  <si>
-    <t>b6</t>
-  </si>
-  <si>
-    <t>b7</t>
-  </si>
-  <si>
-    <t>Saw Wave</t>
-  </si>
-  <si>
     <t>b11 - b8</t>
   </si>
   <si>
@@ -568,6 +535,52 @@
   </si>
   <si>
     <t>波形步长控制</t>
+  </si>
+  <si>
+    <t>WAVFORMQ</t>
+  </si>
+  <si>
+    <t>WAVFORMI</t>
+  </si>
+  <si>
+    <t>b7-b6</t>
+  </si>
+  <si>
+    <t>b5-b4</t>
+  </si>
+  <si>
+    <t>I波形控制</t>
+  </si>
+  <si>
+    <t>Q波形控制</t>
+  </si>
+  <si>
+    <t>DAC使能控制
+，为0时DAC掉电，为1时正常工作</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Rect</t>
+  </si>
+  <si>
+    <t>Saw</t>
+  </si>
+  <si>
+    <t>直流</t>
+  </si>
+  <si>
+    <t>矩形波</t>
+  </si>
+  <si>
+    <t>锯齿波</t>
+  </si>
+  <si>
+    <t>正弦波</t>
+  </si>
+  <si>
+    <t>Cos</t>
   </si>
 </sst>
 </file>
@@ -606,7 +619,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -629,51 +642,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -686,25 +659,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1094,17 +1062,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2131,7 +2099,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2145,7 +2113,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2157,7 +2125,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2169,33 +2137,33 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -2240,7 +2208,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2249,39 +2217,39 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2298,7 +2266,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2313,7 +2281,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2373,13 +2341,13 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2389,17 +2357,17 @@
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2409,17 +2377,17 @@
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2429,189 +2397,199 @@
       <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:A4"/>
@@ -2628,16 +2606,6 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2645,75 +2613,78 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
     <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="21.7109375" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="7" t="s">
+      <c r="P1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" s="7"/>
       <c r="K2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2726,33 +2697,36 @@
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="R2" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="8"/>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="J3" s="4"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="7"/>
       <c r="K3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2765,33 +2739,36 @@
       <c r="N3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="R3" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6" t="s">
+      <c r="O3" s="9"/>
+      <c r="P3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J4" s="4"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="7"/>
       <c r="K4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2802,264 +2779,311 @@
         <v>146</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="R4" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="8" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="R5" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="P5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="7" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="8" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="7" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="8" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="7" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="F11:K11"/>
-    <mergeCell ref="F12:K12"/>
+  <mergeCells count="33">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B16:N16"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B16:K16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented IP with DDS core
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="固件寄存器格式 - 修改" sheetId="4" r:id="rId5"/>
     <sheet name="固件寄存器格式2.00" sheetId="6" r:id="rId6"/>
     <sheet name="固件寄存器格式2.00 - 改" sheetId="8" r:id="rId7"/>
+    <sheet name="固件寄存器格式3.00" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="180">
   <si>
     <t>MSB</t>
   </si>
@@ -581,6 +582,32 @@
   </si>
   <si>
     <t>Cos</t>
+  </si>
+  <si>
+    <t>reg4
+FREQ_CTL
+频率控制寄存器</t>
+  </si>
+  <si>
+    <t>FREQ_CTL_Q</t>
+  </si>
+  <si>
+    <t>Q频率控制</t>
+  </si>
+  <si>
+    <t>b15-b0</t>
+  </si>
+  <si>
+    <t>FREQ_CTL_I</t>
+  </si>
+  <si>
+    <t>I频率控制</t>
+  </si>
+  <si>
+    <t>FREQ_CTL</t>
+  </si>
+  <si>
+    <t>频率控制</t>
   </si>
 </sst>
 </file>
@@ -619,7 +646,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -642,11 +669,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -673,6 +737,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1062,17 +1141,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2099,7 +2178,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2113,7 +2192,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2125,7 +2204,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2137,33 +2216,33 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -2208,7 +2287,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2217,39 +2296,39 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2266,7 +2345,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2281,7 +2360,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2341,13 +2420,13 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2357,17 +2436,17 @@
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2377,17 +2456,17 @@
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2397,199 +2476,189 @@
       <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="8"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="8"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="13" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="8"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="8"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="13" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="8"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="8"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:A4"/>
@@ -2606,6 +2675,16 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2615,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2658,33 +2737,33 @@
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2709,24 +2788,24 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="J3" s="7"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2751,24 +2830,24 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2793,26 +2872,26 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
       <c r="P5" s="6" t="s">
         <v>153</v>
       </c>
@@ -2824,240 +2903,244 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="8"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="8"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="13" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="8"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="8"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="13" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="8"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="8"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B16:N16"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A2:A4"/>
@@ -3068,22 +3151,487 @@
     <mergeCell ref="C8:N8"/>
     <mergeCell ref="C9:N9"/>
     <mergeCell ref="C10:N10"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F11:N11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B14:N14"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="B16:N16"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="P5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="13"/>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="13"/>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="13"/>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I15:N15"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Failed to generate arbitary waveform with BRAM
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="182">
   <si>
     <t>MSB</t>
   </si>
@@ -584,37 +584,43 @@
     <t>Cos</t>
   </si>
   <si>
+    <t>b15-b0</t>
+  </si>
+  <si>
+    <t>FREQ_CTL_I</t>
+  </si>
+  <si>
+    <t>I频率控制</t>
+  </si>
+  <si>
+    <t>FREQ_CTL</t>
+  </si>
+  <si>
+    <t>频率控制</t>
+  </si>
+  <si>
+    <t>b11-b8</t>
+  </si>
+  <si>
+    <t>b15-b12</t>
+  </si>
+  <si>
     <t>reg4
-FREQ_CTL
-频率控制寄存器</t>
-  </si>
-  <si>
-    <t>FREQ_CTL_Q</t>
-  </si>
-  <si>
-    <t>Q频率控制</t>
-  </si>
-  <si>
-    <t>b15-b0</t>
-  </si>
-  <si>
-    <t>FREQ_CTL_I</t>
-  </si>
-  <si>
-    <t>I频率控制</t>
-  </si>
-  <si>
-    <t>FREQ_CTL</t>
-  </si>
-  <si>
-    <t>频率控制</t>
+ARB_DATA
+任意数据寄存器</t>
+  </si>
+  <si>
+    <t>BRAM_ADDR</t>
+  </si>
+  <si>
+    <t>数据地址</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +642,14 @@
       <name val="Symbol"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -710,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -724,12 +738,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,15 +751,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1141,17 +1176,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2178,7 +2213,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2192,7 +2227,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2239,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2216,33 +2251,33 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -2287,7 +2322,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2296,39 +2331,39 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2345,7 +2380,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2360,7 +2395,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2420,13 +2455,13 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2436,17 +2471,17 @@
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2456,17 +2491,17 @@
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="12"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2476,189 +2511,199 @@
       <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:A4"/>
@@ -2675,16 +2720,6 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2737,33 +2772,33 @@
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="J2" s="12"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2776,7 +2811,7 @@
       <c r="N2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="9"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="6" t="s">
         <v>150</v>
       </c>
@@ -2788,24 +2823,24 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="10"/>
       <c r="K3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2818,7 +2853,7 @@
       <c r="N3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="6" t="s">
         <v>151</v>
       </c>
@@ -2830,24 +2865,24 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2860,7 +2895,7 @@
       <c r="N4" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="O4" s="10"/>
+      <c r="O4" s="8"/>
       <c r="P4" s="6" t="s">
         <v>152</v>
       </c>
@@ -2872,275 +2907,271 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
       <c r="P5" s="6" t="s">
         <v>153</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="13"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="13"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="13"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="F11:N11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B14:N14"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B16:N16"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A2:A4"/>
@@ -3156,13 +3187,17 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B16:N16"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3172,447 +3207,461 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="13" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="13" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="13"/>
+    <col min="17" max="17" width="20.7109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="13"/>
+    <col min="19" max="19" width="13.7109375" style="13" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="1" t="s">
+      <c r="C2" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="12" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="12" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="1" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="20"/>
+      <c r="P3" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="12" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="24"/>
+      <c r="P4" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="P5" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="15"/>
+      <c r="B6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="15"/>
+      <c r="B7" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="15"/>
+      <c r="B9" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="15"/>
+      <c r="B10" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="15"/>
+      <c r="B12" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="15"/>
+      <c r="B13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="P5" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="13"/>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="13"/>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="13"/>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="13"/>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="B14" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="13"/>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="13"/>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="13" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="16"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I15:N15"/>
+  <mergeCells count="36">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:N8"/>
     <mergeCell ref="C9:N9"/>
@@ -3623,15 +3672,16 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I15:N15"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="F13:N13"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Trying to improve the clock freqency
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8925" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="信息传输阶段数据格式" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="固件寄存器格式2.00" sheetId="6" r:id="rId6"/>
     <sheet name="固件寄存器格式2.00 - 改" sheetId="8" r:id="rId7"/>
     <sheet name="固件寄存器格式3.00" sheetId="9" r:id="rId8"/>
+    <sheet name="固件寄存器格式3.10" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="198">
   <si>
     <t>MSB</t>
   </si>
@@ -614,6 +615,66 @@
   </si>
   <si>
     <t>数据地址</t>
+  </si>
+  <si>
+    <t>reg1
+DAC_SPI
+DAC SPI寄存器</t>
+  </si>
+  <si>
+    <t>reg2
+ARB_DATA
+任意数据寄存器</t>
+  </si>
+  <si>
+    <t>reg3
+DAC_I_DATA
+DAC I数据寄存器</t>
+  </si>
+  <si>
+    <t>reg4
+DAC_Q_DATA
+DAC Q数据寄存器</t>
+  </si>
+  <si>
+    <t>reg5
+DAC_I_FREQ
+DAC I频率寄存器</t>
+  </si>
+  <si>
+    <t>b31-b0</t>
+  </si>
+  <si>
+    <t>I_FREQ</t>
+  </si>
+  <si>
+    <t>I DAC频率控制字</t>
+  </si>
+  <si>
+    <t>reg6
+DAC_Q_FREQ
+DAC Q频率寄存器</t>
+  </si>
+  <si>
+    <t>Q_FREQ</t>
+  </si>
+  <si>
+    <t>Q DAC频率控制字</t>
+  </si>
+  <si>
+    <t>Arb</t>
+  </si>
+  <si>
+    <t>任意波</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>SIMUL</t>
+  </si>
+  <si>
+    <t>协同控制模式</t>
   </si>
 </sst>
 </file>
@@ -724,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -745,29 +806,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -787,6 +827,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1176,17 +1244,17 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2213,7 +2281,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2227,7 +2295,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="11"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2239,7 +2307,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A4" s="11"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2251,33 +2319,33 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -2322,7 +2390,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2331,39 +2399,39 @@
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="11"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="11"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2380,7 +2448,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="11"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -2395,7 +2463,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="11"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2455,13 +2523,13 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2471,17 +2539,17 @@
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2491,17 +2559,17 @@
       <c r="F3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2511,186 +2579,186 @@
       <c r="F4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="23" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="11"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="23" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="11"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="11"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="23" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="11"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="11"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -2772,33 +2840,33 @@
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
+      <c r="H2" s="22"/>
+      <c r="I2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="1" t="s">
         <v>139</v>
       </c>
@@ -2823,24 +2891,24 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="J3" s="10"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="1" t="s">
         <v>140</v>
       </c>
@@ -2865,24 +2933,24 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2907,26 +2975,26 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="23" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
       <c r="P5" s="6" t="s">
         <v>153</v>
       </c>
@@ -2938,230 +3006,230 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="11"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="11"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="23" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="11"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="11"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="23" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="11"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="11"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -3207,449 +3275,445 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="13" customWidth="1"/>
-    <col min="6" max="7" width="7.85546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="11" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" style="13" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="13"/>
-    <col min="17" max="17" width="20.7109375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="13"/>
-    <col min="19" max="19" width="13.7109375" style="13" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="19.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="11" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="11" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="11"/>
+    <col min="17" max="17" width="20.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="11"/>
+    <col min="19" max="19" width="13.7109375" style="11" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="12" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="21" t="s">
+      <c r="O2" s="13"/>
+      <c r="P2" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="10" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="15"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="12" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="12" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="21" t="s">
+      <c r="O4" s="17"/>
+      <c r="P4" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="10" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="P5" s="21" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="P5" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="R5" s="19" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="15"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="15"/>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="15"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="15"/>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="15"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="15"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="16" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="18"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="16" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="16" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="I2:J2"/>
@@ -3662,6 +3726,23 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I15:N15"/>
+    <mergeCell ref="I16:N16"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:N8"/>
     <mergeCell ref="C9:N9"/>
@@ -3669,19 +3750,639 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:N11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="C13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="11" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="11" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="11" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="11"/>
+    <col min="17" max="17" width="20.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="11"/>
+    <col min="19" max="19" width="13.7109375" style="11" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="25"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1">
+      <c r="A5" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1">
+      <c r="A8" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1">
+      <c r="A10" s="25"/>
+      <c r="B10" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="25"/>
+      <c r="B12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="25"/>
+      <c r="B13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="25"/>
+      <c r="B15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="25"/>
+      <c r="B16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="24"/>
+      <c r="B18" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="24"/>
+      <c r="B19" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="24"/>
+      <c r="B21" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="24"/>
+      <c r="B22" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="C13:N13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I15:N15"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:N5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:N6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="B18:N18"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:N20"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="B22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating driver to support the  full control of 2 channels
</commit_message>
<xml_diff>
--- a/documents/BR0101固件开发——模数转换器 - 表格.xlsx
+++ b/documents/BR0101固件开发——模数转换器 - 表格.xlsx
@@ -835,9 +835,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -847,6 +844,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3321,31 +3321,31 @@
       <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="10" t="s">
         <v>139</v>
       </c>
@@ -3370,22 +3370,22 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="10" t="s">
         <v>140</v>
       </c>
@@ -3410,22 +3410,22 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="10" t="s">
         <v>144</v>
       </c>
@@ -3450,26 +3450,26 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>128</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
       <c r="P5" s="14" t="s">
         <v>153</v>
       </c>
@@ -3481,236 +3481,236 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="25"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="26" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="28"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="26" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="28"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="26" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="28"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -3726,6 +3726,8 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="C13:E13"/>
@@ -3734,8 +3736,13 @@
     <mergeCell ref="C5:N5"/>
     <mergeCell ref="C6:N6"/>
     <mergeCell ref="C7:N7"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:N11"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="B15:H15"/>
@@ -3743,13 +3750,6 @@
     <mergeCell ref="I14:N14"/>
     <mergeCell ref="I15:N15"/>
     <mergeCell ref="I16:N16"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3759,8 +3759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3805,33 +3805,33 @@
       <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
       <c r="K2" s="10" t="s">
         <v>139</v>
       </c>
@@ -3856,22 +3856,22 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="18"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="10" t="s">
         <v>140</v>
       </c>
@@ -3896,22 +3896,22 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="18"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="10" t="s">
         <v>144</v>
       </c>
@@ -3942,22 +3942,22 @@
       <c r="B5" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
       <c r="O5" s="17"/>
       <c r="P5" s="14">
         <v>3</v>
@@ -3970,26 +3970,26 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
       <c r="O6" s="17"/>
       <c r="P6" s="14">
         <v>4</v>
@@ -4002,26 +4002,26 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
       <c r="O7" s="17"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="10"/>
@@ -4031,71 +4031,71 @@
       <c r="A8" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
       <c r="O8" s="17"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
       <c r="O9" s="17"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
       <c r="O10" s="17"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="10"/>
@@ -4108,60 +4108,60 @@
       <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="25"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="29" t="s">
@@ -4170,60 +4170,60 @@
       <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="29" t="s">
@@ -4232,54 +4232,54 @@
       <c r="B17" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="24"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="24"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="29" t="s">
@@ -4288,54 +4288,54 @@
       <c r="B20" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="24"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="24"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="44">

</xml_diff>